<commit_message>
Finish the Week 5 lab practical
</commit_message>
<xml_diff>
--- a/data/wren_trees.xlsx
+++ b/data/wren_trees.xlsx
@@ -49,6 +49,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -133,14 +134,14 @@
   <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.47"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -160,58 +161,58 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>28.2</v>
+        <v>38.2</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>8.6</v>
+        <v>18.6</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>78.1</v>
+        <v>88.1</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>46.5</v>
+        <v>56.5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>20.7</v>
+        <v>30.7</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>9.3</v>
+        <v>19.3</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>49.3</v>
+        <v>59.3</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>46.7</v>
+        <v>56.7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>40.8</v>
+        <v>50.8</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>18.3</v>
+        <v>28.3</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>44.1</v>
+        <v>54.1</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>35.4</v>
+        <v>45.4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>31.7</v>
+        <v>41.7</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>17.2</v>
+        <v>27.2</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>51.6</v>
+        <v>61.6</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>4</v>
@@ -219,480 +220,480 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>12.7</v>
+        <v>22.7</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>36.3</v>
+        <v>46.3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>25.3</v>
+        <v>35.3</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>11.6</v>
+        <v>21.6</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>38.1</v>
+        <v>48.1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>24.8</v>
+        <v>34.8</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>14.9</v>
+        <v>24.9</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>48.5</v>
+        <v>58.5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>30.9</v>
+        <v>40.9</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>13.3</v>
+        <v>23.3</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>50.3</v>
+        <v>60.3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>14.9</v>
+        <v>24.9</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>14.8</v>
+        <v>24.8</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>34.1</v>
+        <v>44.1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>18.3</v>
+        <v>28.3</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>8.2</v>
+        <v>18.2</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>70.3</v>
+        <v>80.3</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>31.2</v>
+        <v>41.2</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>55.1</v>
+        <v>65.1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>24.3</v>
+        <v>34.3</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>14.4</v>
+        <v>24.4</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>55.7</v>
+        <v>65.7</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>20.6</v>
+        <v>30.6</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>13.5</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>29.7</v>
+        <v>39.7</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>13.8</v>
+        <v>23.8</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>23.7</v>
+        <v>33.7</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>13.5</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>34.6</v>
+        <v>44.6</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>11.6</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>22.5</v>
+        <v>32.5</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>29.4</v>
+        <v>39.4</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>17.2</v>
+        <v>27.2</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>35.9</v>
+        <v>45.9</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>13.1</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>22.5</v>
+        <v>32.5</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>14.2</v>
+        <v>24.2</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>15.4</v>
+        <v>25.4</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>8.4</v>
+        <v>18.4</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>24.2</v>
+        <v>34.2</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>6.3</v>
+        <v>16.3</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>35.7</v>
+        <v>45.7</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>28.5</v>
+        <v>38.5</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>31.8</v>
+        <v>41.8</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>22.1</v>
+        <v>32.1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>16.9</v>
+        <v>26.9</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>34.1</v>
+        <v>44.1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>32.9</v>
+        <v>42.9</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>27.8</v>
+        <v>37.8</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>23.8</v>
+        <v>33.8</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>31.3</v>
+        <v>41.3</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>38.4</v>
+        <v>48.4</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>35.6</v>
+        <v>45.6</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>14.3</v>
+        <v>24.3</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>31.3</v>
+        <v>41.3</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>30.7</v>
+        <v>40.7</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>42.5</v>
+        <v>52.5</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
-        <v>32.6</v>
+        <v>42.6</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
-        <v>37.2</v>
+        <v>47.2</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
-        <v>37.4</v>
+        <v>47.4</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
-        <v>20.8</v>
+        <v>30.8</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
-        <v>40.2</v>
+        <v>50.2</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
-        <v>25.2</v>
+        <v>35.2</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
-        <v>23.9</v>
+        <v>33.9</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
-        <v>20.3</v>
+        <v>30.3</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
-        <v>27.7</v>
+        <v>37.7</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
-        <v>29.3</v>
+        <v>39.3</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
-        <v>34.9</v>
+        <v>44.9</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
-        <v>24.8</v>
+        <v>34.8</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
-        <v>36.5</v>
+        <v>46.5</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
-        <v>36.2</v>
+        <v>46.2</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
-        <v>23.8</v>
+        <v>33.8</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
-        <v>22.7</v>
+        <v>32.7</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
-        <v>35.4</v>
+        <v>45.4</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
-        <v>25.5</v>
+        <v>35.5</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
-        <v>27.1</v>
+        <v>37.1</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
-        <v>31.1</v>
+        <v>41.1</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
-        <v>39.3</v>
+        <v>49.3</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
-        <v>24.6</v>
+        <v>34.6</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
-        <v>29.4</v>
+        <v>39.4</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
-        <v>24.3</v>
+        <v>34.3</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
-        <v>33.2</v>
+        <v>43.2</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
-        <v>23.8</v>
+        <v>33.8</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
-        <v>25.4</v>
+        <v>35.4</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
-        <v>28.4</v>
+        <v>38.4</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
-        <v>14.8</v>
+        <v>24.8</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
-        <v>27.1</v>
+        <v>37.1</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
-        <v>32.1</v>
+        <v>42.1</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
-        <v>27.8</v>
+        <v>37.8</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
-        <v>35.8</v>
+        <v>45.8</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
-        <v>36.5</v>
+        <v>46.5</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
-        <v>19.7</v>
+        <v>29.7</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
-        <v>15.9</v>
+        <v>25.9</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
-        <v>14.6</v>
+        <v>24.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix some of the datasets and images and redo the Week5 practical
</commit_message>
<xml_diff>
--- a/data/wren_trees.xlsx
+++ b/data/wren_trees.xlsx
@@ -116,33 +116,32 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="9.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.47"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -167,7 +166,7 @@
         <v>18.6</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>88.1</v>
+        <v>59.3</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>56.5</v>
@@ -181,7 +180,7 @@
         <v>19.3</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>59.3</v>
+        <v>54.1</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>56.7</v>
@@ -195,7 +194,7 @@
         <v>28.3</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>54.1</v>
+        <v>61.6</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>45.4</v>
@@ -209,7 +208,7 @@
         <v>27.2</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>61.6</v>
+        <v>46.3</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>42</v>
@@ -226,7 +225,7 @@
         <v>22.7</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>46.3</v>
+        <v>48.1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -237,7 +236,7 @@
         <v>21.6</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>48.1</v>
+        <v>58.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -248,7 +247,7 @@
         <v>24.9</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>58.5</v>
+        <v>60.3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -259,7 +258,7 @@
         <v>23.3</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>60.3</v>
+        <v>44.1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -270,7 +269,7 @@
         <v>24.8</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>44.1</v>
+        <v>65.1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -281,7 +280,7 @@
         <v>18.2</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>80.3</v>
+        <v>65.7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -291,9 +290,6 @@
       <c r="B12" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="C12" s="0" t="n">
-        <v>65.1</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -302,9 +298,6 @@
       <c r="B13" s="0" t="n">
         <v>24.4</v>
       </c>
-      <c r="C13" s="0" t="n">
-        <v>65.7</v>
-      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -699,7 +692,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>